<commit_message>
:sparkles: Add populating data process
</commit_message>
<xml_diff>
--- a/utils/usuarios.xlsx
+++ b/utils/usuarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="CONSUMOS MACRO 4 "/>
@@ -61,6 +61,9 @@
     <t>CONSUMOS  = MACRO 6 - MACRO 7 - MACRO 8</t>
   </si>
   <si>
+    <t>Shape</t>
+  </si>
+  <si>
     <t xml:space="preserve">MACRO 5 - CONSUMO MACRO 6 = MACRO 6 </t>
   </si>
   <si>
@@ -80,9 +83,6 @@
     <t>MACRO 1 = MACRO 2 (VOLUMEN, EN  DIA, EN UNA SEMAN O EN UN MES), QUE PERMITA AHCER EVALUCIONES</t>
   </si>
   <si>
-    <t>Demanda (l/S)</t>
-  </si>
-  <si>
     <t xml:space="preserve">EL MACRO MEDIDOR 4 LA LECTURA MENSUAL DEBE DE SER IGUAL A LA SUMA DE LOS 93 USUARIOS </t>
   </si>
 </sst>
@@ -91,7 +91,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -135,25 +141,25 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -165,22 +171,22 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -511,12 +517,12 @@
     <col min="15" max="15" style="17" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18" customFormat="1" s="13">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="28.5" customFormat="1" s="13">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>5</v>
@@ -537,7 +543,7 @@
         <v>10</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>12</v>
@@ -550,7 +556,7 @@
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6">
         <v>13</v>
       </c>
@@ -587,7 +593,7 @@
       <c r="N2" s="12"/>
       <c r="O2" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="6">
         <v>14</v>
       </c>
@@ -624,7 +630,7 @@
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="6">
         <v>15</v>
       </c>
@@ -661,7 +667,7 @@
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="6">
         <v>16</v>
       </c>
@@ -698,7 +704,7 @@
       <c r="N5" s="12"/>
       <c r="O5" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="6">
         <v>17</v>
       </c>
@@ -735,7 +741,7 @@
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="6">
         <v>18</v>
       </c>
@@ -772,7 +778,7 @@
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="6">
         <v>19</v>
       </c>
@@ -809,7 +815,7 @@
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="6">
         <v>20</v>
       </c>
@@ -846,7 +852,7 @@
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="6">
         <v>21</v>
       </c>
@@ -883,7 +889,7 @@
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="6">
         <v>22</v>
       </c>
@@ -920,7 +926,7 @@
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="6">
         <v>23</v>
       </c>
@@ -957,7 +963,7 @@
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="6">
         <v>24</v>
       </c>
@@ -994,7 +1000,7 @@
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="6">
         <v>25</v>
       </c>
@@ -1031,7 +1037,7 @@
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="6">
         <v>26</v>
       </c>
@@ -1068,7 +1074,7 @@
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="6">
         <v>27</v>
       </c>
@@ -1105,7 +1111,7 @@
       <c r="N16" s="15"/>
       <c r="O16" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="6">
         <v>28</v>
       </c>
@@ -1142,7 +1148,7 @@
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="6">
         <v>29</v>
       </c>
@@ -1179,7 +1185,7 @@
       <c r="N18" s="15"/>
       <c r="O18" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="6">
         <v>30</v>
       </c>
@@ -1216,7 +1222,7 @@
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="6">
         <v>31</v>
       </c>
@@ -1253,7 +1259,7 @@
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="6">
         <v>32</v>
       </c>
@@ -1290,7 +1296,7 @@
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="6">
         <v>38</v>
       </c>
@@ -1327,7 +1333,7 @@
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="6">
         <v>94</v>
       </c>
@@ -1364,7 +1370,7 @@
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="6">
         <v>95</v>
       </c>
@@ -1401,7 +1407,7 @@
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="6">
         <v>96</v>
       </c>
@@ -1438,7 +1444,7 @@
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="6">
         <v>97</v>
       </c>
@@ -1475,7 +1481,7 @@
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="6">
         <v>99</v>
       </c>
@@ -1512,7 +1518,7 @@
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="6">
         <v>226</v>
       </c>
@@ -4033,7 +4039,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -4061,7 +4067,7 @@
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -4291,7 +4297,7 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -4445,7 +4451,7 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
@@ -4637,7 +4643,7 @@
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
@@ -5954,7 +5960,7 @@
   </sheetPr>
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5980,7 +5986,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -6008,7 +6014,7 @@
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -6195,7 +6201,7 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -8696,7 +8702,7 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8708,7 +8714,7 @@
     <col min="6" max="6" style="10" width="13.005" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="10" width="13.005" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="13.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="8" width="13.005" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="9" width="13.005" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="9" width="13.005" customWidth="1" bestFit="1"/>
@@ -11025,7 +11031,7 @@
       <c r="H61" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I61" s="6" t="s">
+      <c r="I61" s="7" t="s">
         <v>11</v>
       </c>
       <c r="J61" s="6" t="s">

</xml_diff>